<commit_message>
Added population and voting data from censu bureau
</commit_message>
<xml_diff>
--- a/data/family_farmer_estimates.xlsx
+++ b/data/family_farmer_estimates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>State</t>
   </si>
@@ -47,6 +47,78 @@
   </si>
   <si>
     <t>Farmers_in_animal_ag_feed_2012</t>
+  </si>
+  <si>
+    <t>Total_population_2018</t>
+  </si>
+  <si>
+    <t>Total_Citizen_Population_2018</t>
+  </si>
+  <si>
+    <t>Total_Registered_2018</t>
+  </si>
+  <si>
+    <t>Percent_Registered_Total_2018</t>
+  </si>
+  <si>
+    <t>Total_Registered_Margin_of_Error_2018</t>
+  </si>
+  <si>
+    <t>Percent_Registered_Citizen_2018</t>
+  </si>
+  <si>
+    <t>Citizen_Registered_Margin_of_Error_2018</t>
+  </si>
+  <si>
+    <t>Total_Voted_2018</t>
+  </si>
+  <si>
+    <t>Percent_Voted_Total_2018</t>
+  </si>
+  <si>
+    <t>Total_Voted_Margin_of_Error_2018</t>
+  </si>
+  <si>
+    <t>Percent_Voted_Citizen_2018</t>
+  </si>
+  <si>
+    <t>Citizen_Voted_Margin_of_Error_2018</t>
+  </si>
+  <si>
+    <t>Total_population_2012</t>
+  </si>
+  <si>
+    <t>Total_Citizen_Population_2012</t>
+  </si>
+  <si>
+    <t>Total_Registered_2012</t>
+  </si>
+  <si>
+    <t>Percent_Registered_Total_2012</t>
+  </si>
+  <si>
+    <t>Total_Registered_Margin_of_Error_2012</t>
+  </si>
+  <si>
+    <t>Percent_Registered_Citizen_2012</t>
+  </si>
+  <si>
+    <t>Citizen_Registered_Margin_of_Error_2012</t>
+  </si>
+  <si>
+    <t>Total_Voted_2012</t>
+  </si>
+  <si>
+    <t>Percent_Voted_Total_2012</t>
+  </si>
+  <si>
+    <t>Total_Voted_Margin_of_Error_2012</t>
+  </si>
+  <si>
+    <t>Percent_Voted_Citizen_2012</t>
+  </si>
+  <si>
+    <t>Citizen_Voted_Margin_of_Error_2012</t>
   </si>
   <si>
     <t>United States</t>
@@ -557,13 +629,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:AI52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,10 +669,82 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>0.4739383972067674</v>
@@ -632,10 +776,82 @@
       <c r="K2">
         <v>1148042</v>
       </c>
+      <c r="L2">
+        <v>249748</v>
+      </c>
+      <c r="M2">
+        <v>228832000</v>
+      </c>
+      <c r="N2">
+        <v>153066000</v>
+      </c>
+      <c r="O2">
+        <v>61.3</v>
+      </c>
+      <c r="P2">
+        <v>0.3</v>
+      </c>
+      <c r="Q2">
+        <v>66.90000000000001</v>
+      </c>
+      <c r="R2">
+        <v>0.3</v>
+      </c>
+      <c r="S2">
+        <v>122281000</v>
+      </c>
+      <c r="T2">
+        <v>49</v>
+      </c>
+      <c r="U2">
+        <v>0.3</v>
+      </c>
+      <c r="V2">
+        <v>53.4</v>
+      </c>
+      <c r="W2">
+        <v>0.3</v>
+      </c>
+      <c r="X2">
+        <v>235248</v>
+      </c>
+      <c r="Y2">
+        <v>215081000</v>
+      </c>
+      <c r="Z2">
+        <v>153157000</v>
+      </c>
+      <c r="AA2">
+        <v>65.09999999999999</v>
+      </c>
+      <c r="AB2">
+        <v>0.3</v>
+      </c>
+      <c r="AC2">
+        <v>71.2</v>
+      </c>
+      <c r="AD2">
+        <v>0.3</v>
+      </c>
+      <c r="AE2">
+        <v>132948000</v>
+      </c>
+      <c r="AF2">
+        <v>56.5</v>
+      </c>
+      <c r="AG2">
+        <v>0.3</v>
+      </c>
+      <c r="AH2">
+        <v>61.8</v>
+      </c>
+      <c r="AI2">
+        <v>0.3</v>
+      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>0.7931741320940013</v>
@@ -667,10 +883,82 @@
       <c r="K3">
         <v>31320</v>
       </c>
+      <c r="L3">
+        <v>3753</v>
+      </c>
+      <c r="M3">
+        <v>3609000</v>
+      </c>
+      <c r="N3">
+        <v>2490000</v>
+      </c>
+      <c r="O3">
+        <v>66.40000000000001</v>
+      </c>
+      <c r="P3">
+        <v>2.5</v>
+      </c>
+      <c r="Q3">
+        <v>69</v>
+      </c>
+      <c r="R3">
+        <v>2.5</v>
+      </c>
+      <c r="S3">
+        <v>1830000</v>
+      </c>
+      <c r="T3">
+        <v>48.8</v>
+      </c>
+      <c r="U3">
+        <v>2.7</v>
+      </c>
+      <c r="V3">
+        <v>50.7</v>
+      </c>
+      <c r="W3">
+        <v>2.7</v>
+      </c>
+      <c r="X3">
+        <v>3594</v>
+      </c>
+      <c r="Y3">
+        <v>3479000</v>
+      </c>
+      <c r="Z3">
+        <v>2556000</v>
+      </c>
+      <c r="AA3">
+        <v>71.09999999999999</v>
+      </c>
+      <c r="AB3">
+        <v>2.2</v>
+      </c>
+      <c r="AC3">
+        <v>73.5</v>
+      </c>
+      <c r="AD3">
+        <v>2.2</v>
+      </c>
+      <c r="AE3">
+        <v>2154000</v>
+      </c>
+      <c r="AF3">
+        <v>59.9</v>
+      </c>
+      <c r="AG3">
+        <v>2.4</v>
+      </c>
+      <c r="AH3">
+        <v>61.9</v>
+      </c>
+      <c r="AI3">
+        <v>2.4</v>
+      </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:35">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B4">
         <v>0.1851368600198553</v>
@@ -702,10 +990,82 @@
       <c r="K4">
         <v>259</v>
       </c>
+      <c r="L4">
+        <v>523</v>
+      </c>
+      <c r="M4">
+        <v>497000</v>
+      </c>
+      <c r="N4">
+        <v>337000</v>
+      </c>
+      <c r="O4">
+        <v>64.40000000000001</v>
+      </c>
+      <c r="P4">
+        <v>2.7</v>
+      </c>
+      <c r="Q4">
+        <v>67.7</v>
+      </c>
+      <c r="R4">
+        <v>2.7</v>
+      </c>
+      <c r="S4">
+        <v>263000</v>
+      </c>
+      <c r="T4">
+        <v>50.2</v>
+      </c>
+      <c r="U4">
+        <v>2.9</v>
+      </c>
+      <c r="V4">
+        <v>52.8</v>
+      </c>
+      <c r="W4">
+        <v>2.9</v>
+      </c>
+      <c r="X4">
+        <v>516</v>
+      </c>
+      <c r="Y4">
+        <v>495000</v>
+      </c>
+      <c r="Z4">
+        <v>361000</v>
+      </c>
+      <c r="AA4">
+        <v>69.90000000000001</v>
+      </c>
+      <c r="AB4">
+        <v>2.4</v>
+      </c>
+      <c r="AC4">
+        <v>72.8</v>
+      </c>
+      <c r="AD4">
+        <v>2.4</v>
+      </c>
+      <c r="AE4">
+        <v>289000</v>
+      </c>
+      <c r="AF4">
+        <v>56</v>
+      </c>
+      <c r="AG4">
+        <v>2.6</v>
+      </c>
+      <c r="AH4">
+        <v>58.4</v>
+      </c>
+      <c r="AI4">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>0.3855619959977147</v>
@@ -737,10 +1097,82 @@
       <c r="K5">
         <v>9224</v>
       </c>
+      <c r="L5">
+        <v>5361</v>
+      </c>
+      <c r="M5">
+        <v>4757000</v>
+      </c>
+      <c r="N5">
+        <v>3262000</v>
+      </c>
+      <c r="O5">
+        <v>60.8</v>
+      </c>
+      <c r="P5">
+        <v>2.2</v>
+      </c>
+      <c r="Q5">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="R5">
+        <v>2.2</v>
+      </c>
+      <c r="S5">
+        <v>2800000</v>
+      </c>
+      <c r="T5">
+        <v>52.2</v>
+      </c>
+      <c r="U5">
+        <v>2.3</v>
+      </c>
+      <c r="V5">
+        <v>58.9</v>
+      </c>
+      <c r="W5">
+        <v>2.4</v>
+      </c>
+      <c r="X5">
+        <v>4863</v>
+      </c>
+      <c r="Y5">
+        <v>4314000</v>
+      </c>
+      <c r="Z5">
+        <v>2812000</v>
+      </c>
+      <c r="AA5">
+        <v>57.8</v>
+      </c>
+      <c r="AB5">
+        <v>2.1</v>
+      </c>
+      <c r="AC5">
+        <v>65.2</v>
+      </c>
+      <c r="AD5">
+        <v>2.2</v>
+      </c>
+      <c r="AE5">
+        <v>2412000</v>
+      </c>
+      <c r="AF5">
+        <v>49.6</v>
+      </c>
+      <c r="AG5">
+        <v>2.2</v>
+      </c>
+      <c r="AH5">
+        <v>55.9</v>
+      </c>
+      <c r="AI5">
+        <v>2.3</v>
+      </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>0.5990452736753897</v>
@@ -772,10 +1204,82 @@
       <c r="K6">
         <v>22320</v>
       </c>
+      <c r="L6">
+        <v>2261</v>
+      </c>
+      <c r="M6">
+        <v>2158000</v>
+      </c>
+      <c r="N6">
+        <v>1262000</v>
+      </c>
+      <c r="O6">
+        <v>55.8</v>
+      </c>
+      <c r="P6">
+        <v>2.7</v>
+      </c>
+      <c r="Q6">
+        <v>58.5</v>
+      </c>
+      <c r="R6">
+        <v>2.8</v>
+      </c>
+      <c r="S6">
+        <v>919000</v>
+      </c>
+      <c r="T6">
+        <v>40.6</v>
+      </c>
+      <c r="U6">
+        <v>2.7</v>
+      </c>
+      <c r="V6">
+        <v>42.6</v>
+      </c>
+      <c r="W6">
+        <v>2.8</v>
+      </c>
+      <c r="X6">
+        <v>2198</v>
+      </c>
+      <c r="Y6">
+        <v>2109000</v>
+      </c>
+      <c r="Z6">
+        <v>1376000</v>
+      </c>
+      <c r="AA6">
+        <v>62.6</v>
+      </c>
+      <c r="AB6">
+        <v>2.4</v>
+      </c>
+      <c r="AC6">
+        <v>65.3</v>
+      </c>
+      <c r="AD6">
+        <v>2.4</v>
+      </c>
+      <c r="AE6">
+        <v>1124000</v>
+      </c>
+      <c r="AF6">
+        <v>51.1</v>
+      </c>
+      <c r="AG6">
+        <v>2.5</v>
+      </c>
+      <c r="AH6">
+        <v>53.3</v>
+      </c>
+      <c r="AI6">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:35">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B7">
         <v>0.2256981700769825</v>
@@ -807,10 +1311,82 @@
       <c r="K7">
         <v>17394</v>
       </c>
+      <c r="L7">
+        <v>30243</v>
+      </c>
+      <c r="M7">
+        <v>25525000</v>
+      </c>
+      <c r="N7">
+        <v>15690000</v>
+      </c>
+      <c r="O7">
+        <v>51.9</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>61.5</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>13240000</v>
+      </c>
+      <c r="T7">
+        <v>43.8</v>
+      </c>
+      <c r="U7">
+        <v>0.9</v>
+      </c>
+      <c r="V7">
+        <v>51.9</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>28357</v>
+      </c>
+      <c r="Y7">
+        <v>23419000</v>
+      </c>
+      <c r="Z7">
+        <v>15356000</v>
+      </c>
+      <c r="AA7">
+        <v>54.2</v>
+      </c>
+      <c r="AB7">
+        <v>0.9</v>
+      </c>
+      <c r="AC7">
+        <v>65.59999999999999</v>
+      </c>
+      <c r="AD7">
+        <v>0.9</v>
+      </c>
+      <c r="AE7">
+        <v>13462000</v>
+      </c>
+      <c r="AF7">
+        <v>47.5</v>
+      </c>
+      <c r="AG7">
+        <v>0.9</v>
+      </c>
+      <c r="AH7">
+        <v>57.5</v>
+      </c>
+      <c r="AI7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:35">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>0.6836241432705691</v>
@@ -842,10 +1418,82 @@
       <c r="K8">
         <v>23918</v>
       </c>
+      <c r="L8">
+        <v>4353</v>
+      </c>
+      <c r="M8">
+        <v>4029000</v>
+      </c>
+      <c r="N8">
+        <v>2645000</v>
+      </c>
+      <c r="O8">
+        <v>60.8</v>
+      </c>
+      <c r="P8">
+        <v>2.5</v>
+      </c>
+      <c r="Q8">
+        <v>65.59999999999999</v>
+      </c>
+      <c r="R8">
+        <v>2.5</v>
+      </c>
+      <c r="S8">
+        <v>2342000</v>
+      </c>
+      <c r="T8">
+        <v>53.8</v>
+      </c>
+      <c r="U8">
+        <v>2.5</v>
+      </c>
+      <c r="V8">
+        <v>58.1</v>
+      </c>
+      <c r="W8">
+        <v>2.6</v>
+      </c>
+      <c r="X8">
+        <v>3817</v>
+      </c>
+      <c r="Y8">
+        <v>3544000</v>
+      </c>
+      <c r="Z8">
+        <v>2635000</v>
+      </c>
+      <c r="AA8">
+        <v>69</v>
+      </c>
+      <c r="AB8">
+        <v>2.3</v>
+      </c>
+      <c r="AC8">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="AD8">
+        <v>2.2</v>
+      </c>
+      <c r="AE8">
+        <v>2495000</v>
+      </c>
+      <c r="AF8">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="AG8">
+        <v>2.3</v>
+      </c>
+      <c r="AH8">
+        <v>70.40000000000001</v>
+      </c>
+      <c r="AI8">
+        <v>2.3</v>
+      </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <v>0.2834475948275718</v>
@@ -877,10 +1525,82 @@
       <c r="K9">
         <v>1557</v>
       </c>
+      <c r="L9">
+        <v>2834</v>
+      </c>
+      <c r="M9">
+        <v>2539000</v>
+      </c>
+      <c r="N9">
+        <v>1726000</v>
+      </c>
+      <c r="O9">
+        <v>60.9</v>
+      </c>
+      <c r="P9">
+        <v>2.6</v>
+      </c>
+      <c r="Q9">
+        <v>68</v>
+      </c>
+      <c r="R9">
+        <v>2.7</v>
+      </c>
+      <c r="S9">
+        <v>1370000</v>
+      </c>
+      <c r="T9">
+        <v>48.3</v>
+      </c>
+      <c r="U9">
+        <v>2.7</v>
+      </c>
+      <c r="V9">
+        <v>54</v>
+      </c>
+      <c r="W9">
+        <v>2.9</v>
+      </c>
+      <c r="X9">
+        <v>2726</v>
+      </c>
+      <c r="Y9">
+        <v>2499000</v>
+      </c>
+      <c r="Z9">
+        <v>1760000</v>
+      </c>
+      <c r="AA9">
+        <v>64.59999999999999</v>
+      </c>
+      <c r="AB9">
+        <v>2.5</v>
+      </c>
+      <c r="AC9">
+        <v>70.40000000000001</v>
+      </c>
+      <c r="AD9">
+        <v>2.5</v>
+      </c>
+      <c r="AE9">
+        <v>1568000</v>
+      </c>
+      <c r="AF9">
+        <v>57.5</v>
+      </c>
+      <c r="AG9">
+        <v>2.5</v>
+      </c>
+      <c r="AH9">
+        <v>62.7</v>
+      </c>
+      <c r="AI9">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <v>0.7942837298401401</v>
@@ -912,10 +1632,82 @@
       <c r="K10">
         <v>1562</v>
       </c>
+      <c r="L10">
+        <v>756</v>
+      </c>
+      <c r="M10">
+        <v>713000</v>
+      </c>
+      <c r="N10">
+        <v>472000</v>
+      </c>
+      <c r="O10">
+        <v>62.4</v>
+      </c>
+      <c r="P10">
+        <v>2.6</v>
+      </c>
+      <c r="Q10">
+        <v>66.3</v>
+      </c>
+      <c r="R10">
+        <v>2.6</v>
+      </c>
+      <c r="S10">
+        <v>369000</v>
+      </c>
+      <c r="T10">
+        <v>48.8</v>
+      </c>
+      <c r="U10">
+        <v>2.7</v>
+      </c>
+      <c r="V10">
+        <v>51.8</v>
+      </c>
+      <c r="W10">
+        <v>2.8</v>
+      </c>
+      <c r="X10">
+        <v>693</v>
+      </c>
+      <c r="Y10">
+        <v>641000</v>
+      </c>
+      <c r="Z10">
+        <v>470000</v>
+      </c>
+      <c r="AA10">
+        <v>67.8</v>
+      </c>
+      <c r="AB10">
+        <v>2.4</v>
+      </c>
+      <c r="AC10">
+        <v>73.3</v>
+      </c>
+      <c r="AD10">
+        <v>2.4</v>
+      </c>
+      <c r="AE10">
+        <v>431000</v>
+      </c>
+      <c r="AF10">
+        <v>62.2</v>
+      </c>
+      <c r="AG10">
+        <v>2.5</v>
+      </c>
+      <c r="AH10">
+        <v>67.3</v>
+      </c>
+      <c r="AI10">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:35">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <v>0.2137016362438832</v>
@@ -947,10 +1739,82 @@
       <c r="K11">
         <v>8588</v>
       </c>
+      <c r="L11">
+        <v>16845</v>
+      </c>
+      <c r="M11">
+        <v>15047000</v>
+      </c>
+      <c r="N11">
+        <v>9435000</v>
+      </c>
+      <c r="O11">
+        <v>56</v>
+      </c>
+      <c r="P11">
+        <v>1.2</v>
+      </c>
+      <c r="Q11">
+        <v>62.7</v>
+      </c>
+      <c r="R11">
+        <v>1.3</v>
+      </c>
+      <c r="S11">
+        <v>7918000</v>
+      </c>
+      <c r="T11">
+        <v>47</v>
+      </c>
+      <c r="U11">
+        <v>1.3</v>
+      </c>
+      <c r="V11">
+        <v>52.6</v>
+      </c>
+      <c r="W11">
+        <v>1.3</v>
+      </c>
+      <c r="X11">
+        <v>15034</v>
+      </c>
+      <c r="Y11">
+        <v>13326000</v>
+      </c>
+      <c r="Z11">
+        <v>9102000</v>
+      </c>
+      <c r="AA11">
+        <v>60.5</v>
+      </c>
+      <c r="AB11">
+        <v>1.2</v>
+      </c>
+      <c r="AC11">
+        <v>68.3</v>
+      </c>
+      <c r="AD11">
+        <v>1.2</v>
+      </c>
+      <c r="AE11">
+        <v>8107000</v>
+      </c>
+      <c r="AF11">
+        <v>53.9</v>
+      </c>
+      <c r="AG11">
+        <v>1.2</v>
+      </c>
+      <c r="AH11">
+        <v>60.8</v>
+      </c>
+      <c r="AI11">
+        <v>1.3</v>
+      </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:35">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="B12">
         <v>0.652430017989594</v>
@@ -982,10 +1846,82 @@
       <c r="K12">
         <v>23034</v>
       </c>
+      <c r="L12">
+        <v>7850</v>
+      </c>
+      <c r="M12">
+        <v>7311000</v>
+      </c>
+      <c r="N12">
+        <v>4840000</v>
+      </c>
+      <c r="O12">
+        <v>61.7</v>
+      </c>
+      <c r="P12">
+        <v>1.8</v>
+      </c>
+      <c r="Q12">
+        <v>66.2</v>
+      </c>
+      <c r="R12">
+        <v>1.8</v>
+      </c>
+      <c r="S12">
+        <v>4084000</v>
+      </c>
+      <c r="T12">
+        <v>52</v>
+      </c>
+      <c r="U12">
+        <v>1.9</v>
+      </c>
+      <c r="V12">
+        <v>55.9</v>
+      </c>
+      <c r="W12">
+        <v>1.9</v>
+      </c>
+      <c r="X12">
+        <v>7179</v>
+      </c>
+      <c r="Y12">
+        <v>6738000</v>
+      </c>
+      <c r="Z12">
+        <v>4767000</v>
+      </c>
+      <c r="AA12">
+        <v>66.40000000000001</v>
+      </c>
+      <c r="AB12">
+        <v>1.7</v>
+      </c>
+      <c r="AC12">
+        <v>70.7</v>
+      </c>
+      <c r="AD12">
+        <v>1.7</v>
+      </c>
+      <c r="AE12">
+        <v>4168000</v>
+      </c>
+      <c r="AF12">
+        <v>58.1</v>
+      </c>
+      <c r="AG12">
+        <v>1.7</v>
+      </c>
+      <c r="AH12">
+        <v>61.9</v>
+      </c>
+      <c r="AI12">
+        <v>1.8</v>
+      </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:35">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>0.2449371803071529</v>
@@ -1017,10 +1953,82 @@
       <c r="K13">
         <v>1037</v>
       </c>
+      <c r="L13">
+        <v>1057</v>
+      </c>
+      <c r="M13">
+        <v>971000</v>
+      </c>
+      <c r="N13">
+        <v>523000</v>
+      </c>
+      <c r="O13">
+        <v>49.5</v>
+      </c>
+      <c r="P13">
+        <v>2.7</v>
+      </c>
+      <c r="Q13">
+        <v>53.9</v>
+      </c>
+      <c r="R13">
+        <v>2.8</v>
+      </c>
+      <c r="S13">
+        <v>427000</v>
+      </c>
+      <c r="T13">
+        <v>40.4</v>
+      </c>
+      <c r="U13">
+        <v>2.7</v>
+      </c>
+      <c r="V13">
+        <v>44</v>
+      </c>
+      <c r="W13">
+        <v>2.8</v>
+      </c>
+      <c r="X13">
+        <v>1013</v>
+      </c>
+      <c r="Y13">
+        <v>930000</v>
+      </c>
+      <c r="Z13">
+        <v>547000</v>
+      </c>
+      <c r="AA13">
+        <v>54.1</v>
+      </c>
+      <c r="AB13">
+        <v>2.4</v>
+      </c>
+      <c r="AC13">
+        <v>58.9</v>
+      </c>
+      <c r="AD13">
+        <v>2.5</v>
+      </c>
+      <c r="AE13">
+        <v>480000</v>
+      </c>
+      <c r="AF13">
+        <v>47.4</v>
+      </c>
+      <c r="AG13">
+        <v>2.4</v>
+      </c>
+      <c r="AH13">
+        <v>51.6</v>
+      </c>
+      <c r="AI13">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:35">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B14">
         <v>0.5964814565035856</v>
@@ -1052,10 +2060,82 @@
       <c r="K14">
         <v>13407</v>
       </c>
+      <c r="L14">
+        <v>1299</v>
+      </c>
+      <c r="M14">
+        <v>1226000</v>
+      </c>
+      <c r="N14">
+        <v>743000</v>
+      </c>
+      <c r="O14">
+        <v>57.2</v>
+      </c>
+      <c r="P14">
+        <v>2.7</v>
+      </c>
+      <c r="Q14">
+        <v>60.6</v>
+      </c>
+      <c r="R14">
+        <v>2.7</v>
+      </c>
+      <c r="S14">
+        <v>587000</v>
+      </c>
+      <c r="T14">
+        <v>45.2</v>
+      </c>
+      <c r="U14">
+        <v>2.7</v>
+      </c>
+      <c r="V14">
+        <v>47.9</v>
+      </c>
+      <c r="W14">
+        <v>2.8</v>
+      </c>
+      <c r="X14">
+        <v>1129</v>
+      </c>
+      <c r="Y14">
+        <v>1064000</v>
+      </c>
+      <c r="Z14">
+        <v>745000</v>
+      </c>
+      <c r="AA14">
+        <v>65.90000000000001</v>
+      </c>
+      <c r="AB14">
+        <v>2.4</v>
+      </c>
+      <c r="AC14">
+        <v>70</v>
+      </c>
+      <c r="AD14">
+        <v>2.3</v>
+      </c>
+      <c r="AE14">
+        <v>679000</v>
+      </c>
+      <c r="AF14">
+        <v>60.2</v>
+      </c>
+      <c r="AG14">
+        <v>2.4</v>
+      </c>
+      <c r="AH14">
+        <v>63.9</v>
+      </c>
+      <c r="AI14">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:35">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>0.1615354636344928</v>
@@ -1087,10 +2167,82 @@
       <c r="K15">
         <v>43261</v>
       </c>
+      <c r="L15">
+        <v>9732</v>
+      </c>
+      <c r="M15">
+        <v>8947000</v>
+      </c>
+      <c r="N15">
+        <v>6068000</v>
+      </c>
+      <c r="O15">
+        <v>62.4</v>
+      </c>
+      <c r="P15">
+        <v>1.6</v>
+      </c>
+      <c r="Q15">
+        <v>67.8</v>
+      </c>
+      <c r="R15">
+        <v>1.6</v>
+      </c>
+      <c r="S15">
+        <v>4740000</v>
+      </c>
+      <c r="T15">
+        <v>48.7</v>
+      </c>
+      <c r="U15">
+        <v>1.7</v>
+      </c>
+      <c r="V15">
+        <v>53</v>
+      </c>
+      <c r="W15">
+        <v>1.7</v>
+      </c>
+      <c r="X15">
+        <v>9651</v>
+      </c>
+      <c r="Y15">
+        <v>8831000</v>
+      </c>
+      <c r="Z15">
+        <v>6425000</v>
+      </c>
+      <c r="AA15">
+        <v>66.59999999999999</v>
+      </c>
+      <c r="AB15">
+        <v>1.4</v>
+      </c>
+      <c r="AC15">
+        <v>72.7</v>
+      </c>
+      <c r="AD15">
+        <v>1.4</v>
+      </c>
+      <c r="AE15">
+        <v>5428000</v>
+      </c>
+      <c r="AF15">
+        <v>56.2</v>
+      </c>
+      <c r="AG15">
+        <v>1.5</v>
+      </c>
+      <c r="AH15">
+        <v>61.5</v>
+      </c>
+      <c r="AI15">
+        <v>1.6</v>
+      </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:35">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B16">
         <v>0.357763733538059</v>
@@ -1122,10 +2274,82 @@
       <c r="K16">
         <v>34440</v>
       </c>
+      <c r="L16">
+        <v>5006</v>
+      </c>
+      <c r="M16">
+        <v>4792000</v>
+      </c>
+      <c r="N16">
+        <v>3131000</v>
+      </c>
+      <c r="O16">
+        <v>62.5</v>
+      </c>
+      <c r="P16">
+        <v>2.2</v>
+      </c>
+      <c r="Q16">
+        <v>65.3</v>
+      </c>
+      <c r="R16">
+        <v>2.3</v>
+      </c>
+      <c r="S16">
+        <v>2364000</v>
+      </c>
+      <c r="T16">
+        <v>47.2</v>
+      </c>
+      <c r="U16">
+        <v>2.3</v>
+      </c>
+      <c r="V16">
+        <v>49.3</v>
+      </c>
+      <c r="W16">
+        <v>2.4</v>
+      </c>
+      <c r="X16">
+        <v>4852</v>
+      </c>
+      <c r="Y16">
+        <v>4724000</v>
+      </c>
+      <c r="Z16">
+        <v>3270000</v>
+      </c>
+      <c r="AA16">
+        <v>67.40000000000001</v>
+      </c>
+      <c r="AB16">
+        <v>2</v>
+      </c>
+      <c r="AC16">
+        <v>69.2</v>
+      </c>
+      <c r="AD16">
+        <v>2</v>
+      </c>
+      <c r="AE16">
+        <v>2801000</v>
+      </c>
+      <c r="AF16">
+        <v>57.7</v>
+      </c>
+      <c r="AG16">
+        <v>2.1</v>
+      </c>
+      <c r="AH16">
+        <v>59.3</v>
+      </c>
+      <c r="AI16">
+        <v>2.1</v>
+      </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:35">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B17">
         <v>0.5056330365168575</v>
@@ -1157,10 +2381,82 @@
       <c r="K17">
         <v>59796</v>
       </c>
+      <c r="L17">
+        <v>2376</v>
+      </c>
+      <c r="M17">
+        <v>2239000</v>
+      </c>
+      <c r="N17">
+        <v>1658000</v>
+      </c>
+      <c r="O17">
+        <v>69.8</v>
+      </c>
+      <c r="P17">
+        <v>2.6</v>
+      </c>
+      <c r="Q17">
+        <v>74</v>
+      </c>
+      <c r="R17">
+        <v>2.5</v>
+      </c>
+      <c r="S17">
+        <v>1335000</v>
+      </c>
+      <c r="T17">
+        <v>56.2</v>
+      </c>
+      <c r="U17">
+        <v>2.8</v>
+      </c>
+      <c r="V17">
+        <v>59.6</v>
+      </c>
+      <c r="W17">
+        <v>2.8</v>
+      </c>
+      <c r="X17">
+        <v>2320</v>
+      </c>
+      <c r="Y17">
+        <v>2232000</v>
+      </c>
+      <c r="Z17">
+        <v>1745000</v>
+      </c>
+      <c r="AA17">
+        <v>75.2</v>
+      </c>
+      <c r="AB17">
+        <v>2.3</v>
+      </c>
+      <c r="AC17">
+        <v>78.2</v>
+      </c>
+      <c r="AD17">
+        <v>2.2</v>
+      </c>
+      <c r="AE17">
+        <v>1548000</v>
+      </c>
+      <c r="AF17">
+        <v>66.7</v>
+      </c>
+      <c r="AG17">
+        <v>2.5</v>
+      </c>
+      <c r="AH17">
+        <v>69.40000000000001</v>
+      </c>
+      <c r="AI17">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:35">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B18">
         <v>0.6095720551653192</v>
@@ -1192,10 +2488,82 @@
       <c r="K18">
         <v>40092</v>
       </c>
+      <c r="L18">
+        <v>2149</v>
+      </c>
+      <c r="M18">
+        <v>2026000</v>
+      </c>
+      <c r="N18">
+        <v>1449000</v>
+      </c>
+      <c r="O18">
+        <v>67.40000000000001</v>
+      </c>
+      <c r="P18">
+        <v>2.8</v>
+      </c>
+      <c r="Q18">
+        <v>71.5</v>
+      </c>
+      <c r="R18">
+        <v>2.8</v>
+      </c>
+      <c r="S18">
+        <v>1152000</v>
+      </c>
+      <c r="T18">
+        <v>53.6</v>
+      </c>
+      <c r="U18">
+        <v>3</v>
+      </c>
+      <c r="V18">
+        <v>56.9</v>
+      </c>
+      <c r="W18">
+        <v>3</v>
+      </c>
+      <c r="X18">
+        <v>2120</v>
+      </c>
+      <c r="Y18">
+        <v>1973000</v>
+      </c>
+      <c r="Z18">
+        <v>1467000</v>
+      </c>
+      <c r="AA18">
+        <v>69.2</v>
+      </c>
+      <c r="AB18">
+        <v>2.4</v>
+      </c>
+      <c r="AC18">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="AD18">
+        <v>2.4</v>
+      </c>
+      <c r="AE18">
+        <v>1249000</v>
+      </c>
+      <c r="AF18">
+        <v>58.9</v>
+      </c>
+      <c r="AG18">
+        <v>2.6</v>
+      </c>
+      <c r="AH18">
+        <v>63.3</v>
+      </c>
+      <c r="AI18">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:35">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>0.5719702478614708</v>
@@ -1227,10 +2595,82 @@
       <c r="K19">
         <v>48913</v>
       </c>
+      <c r="L19">
+        <v>3370</v>
+      </c>
+      <c r="M19">
+        <v>3249000</v>
+      </c>
+      <c r="N19">
+        <v>2389000</v>
+      </c>
+      <c r="O19">
+        <v>70.90000000000001</v>
+      </c>
+      <c r="P19">
+        <v>2.6</v>
+      </c>
+      <c r="Q19">
+        <v>73.5</v>
+      </c>
+      <c r="R19">
+        <v>2.6</v>
+      </c>
+      <c r="S19">
+        <v>1746000</v>
+      </c>
+      <c r="T19">
+        <v>51.8</v>
+      </c>
+      <c r="U19">
+        <v>2.9</v>
+      </c>
+      <c r="V19">
+        <v>53.8</v>
+      </c>
+      <c r="W19">
+        <v>2.9</v>
+      </c>
+      <c r="X19">
+        <v>3291</v>
+      </c>
+      <c r="Y19">
+        <v>3194000</v>
+      </c>
+      <c r="Z19">
+        <v>2303000</v>
+      </c>
+      <c r="AA19">
+        <v>70</v>
+      </c>
+      <c r="AB19">
+        <v>2.4</v>
+      </c>
+      <c r="AC19">
+        <v>72.09999999999999</v>
+      </c>
+      <c r="AD19">
+        <v>2.4</v>
+      </c>
+      <c r="AE19">
+        <v>1895000</v>
+      </c>
+      <c r="AF19">
+        <v>57.6</v>
+      </c>
+      <c r="AG19">
+        <v>2.6</v>
+      </c>
+      <c r="AH19">
+        <v>59.3</v>
+      </c>
+      <c r="AI19">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:35">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>0.3585459374440173</v>
@@ -1262,10 +2702,82 @@
       <c r="K20">
         <v>11095</v>
       </c>
+      <c r="L20">
+        <v>3458</v>
+      </c>
+      <c r="M20">
+        <v>3326000</v>
+      </c>
+      <c r="N20">
+        <v>2263000</v>
+      </c>
+      <c r="O20">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="P20">
+        <v>2.6</v>
+      </c>
+      <c r="Q20">
+        <v>68</v>
+      </c>
+      <c r="R20">
+        <v>2.6</v>
+      </c>
+      <c r="S20">
+        <v>1656000</v>
+      </c>
+      <c r="T20">
+        <v>47.9</v>
+      </c>
+      <c r="U20">
+        <v>2.7</v>
+      </c>
+      <c r="V20">
+        <v>49.8</v>
+      </c>
+      <c r="W20">
+        <v>2.7</v>
+      </c>
+      <c r="X20">
+        <v>3321</v>
+      </c>
+      <c r="Y20">
+        <v>3239000</v>
+      </c>
+      <c r="Z20">
+        <v>2498000</v>
+      </c>
+      <c r="AA20">
+        <v>75.2</v>
+      </c>
+      <c r="AB20">
+        <v>2.2</v>
+      </c>
+      <c r="AC20">
+        <v>77.09999999999999</v>
+      </c>
+      <c r="AD20">
+        <v>2.2</v>
+      </c>
+      <c r="AE20">
+        <v>2148000</v>
+      </c>
+      <c r="AF20">
+        <v>64.7</v>
+      </c>
+      <c r="AG20">
+        <v>2.4</v>
+      </c>
+      <c r="AH20">
+        <v>66.3</v>
+      </c>
+      <c r="AI20">
+        <v>2.4</v>
+      </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:35">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="B21">
         <v>0.422409229177073</v>
@@ -1297,10 +2809,82 @@
       <c r="K21">
         <v>3240</v>
       </c>
+      <c r="L21">
+        <v>1074</v>
+      </c>
+      <c r="M21">
+        <v>1056000</v>
+      </c>
+      <c r="N21">
+        <v>828000</v>
+      </c>
+      <c r="O21">
+        <v>77.09999999999999</v>
+      </c>
+      <c r="P21">
+        <v>2.6</v>
+      </c>
+      <c r="Q21">
+        <v>78.40000000000001</v>
+      </c>
+      <c r="R21">
+        <v>2.5</v>
+      </c>
+      <c r="S21">
+        <v>693000</v>
+      </c>
+      <c r="T21">
+        <v>64.5</v>
+      </c>
+      <c r="U21">
+        <v>2.9</v>
+      </c>
+      <c r="V21">
+        <v>65.59999999999999</v>
+      </c>
+      <c r="W21">
+        <v>2.9</v>
+      </c>
+      <c r="X21">
+        <v>1042</v>
+      </c>
+      <c r="Y21">
+        <v>1020000</v>
+      </c>
+      <c r="Z21">
+        <v>787000</v>
+      </c>
+      <c r="AA21">
+        <v>75.5</v>
+      </c>
+      <c r="AB21">
+        <v>2.4</v>
+      </c>
+      <c r="AC21">
+        <v>77.09999999999999</v>
+      </c>
+      <c r="AD21">
+        <v>2.4</v>
+      </c>
+      <c r="AE21">
+        <v>700000</v>
+      </c>
+      <c r="AF21">
+        <v>67.2</v>
+      </c>
+      <c r="AG21">
+        <v>2.7</v>
+      </c>
+      <c r="AH21">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="AI21">
+        <v>2.7</v>
+      </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:35">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B22">
         <v>0.6027494783462598</v>
@@ -1332,10 +2916,82 @@
       <c r="K22">
         <v>6972</v>
       </c>
+      <c r="L22">
+        <v>4666</v>
+      </c>
+      <c r="M22">
+        <v>4281000</v>
+      </c>
+      <c r="N22">
+        <v>3095000</v>
+      </c>
+      <c r="O22">
+        <v>66.3</v>
+      </c>
+      <c r="P22">
+        <v>2.3</v>
+      </c>
+      <c r="Q22">
+        <v>72.3</v>
+      </c>
+      <c r="R22">
+        <v>2.3</v>
+      </c>
+      <c r="S22">
+        <v>2320000</v>
+      </c>
+      <c r="T22">
+        <v>49.7</v>
+      </c>
+      <c r="U22">
+        <v>2.5</v>
+      </c>
+      <c r="V22">
+        <v>54.2</v>
+      </c>
+      <c r="W22">
+        <v>2.6</v>
+      </c>
+      <c r="X22">
+        <v>4449</v>
+      </c>
+      <c r="Y22">
+        <v>4007000</v>
+      </c>
+      <c r="Z22">
+        <v>2888000</v>
+      </c>
+      <c r="AA22">
+        <v>64.90000000000001</v>
+      </c>
+      <c r="AB22">
+        <v>2.2</v>
+      </c>
+      <c r="AC22">
+        <v>72.09999999999999</v>
+      </c>
+      <c r="AD22">
+        <v>2.2</v>
+      </c>
+      <c r="AE22">
+        <v>2609000</v>
+      </c>
+      <c r="AF22">
+        <v>58.7</v>
+      </c>
+      <c r="AG22">
+        <v>2.2</v>
+      </c>
+      <c r="AH22">
+        <v>65.09999999999999</v>
+      </c>
+      <c r="AI22">
+        <v>2.3</v>
+      </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:35">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B23">
         <v>0.240980669840696</v>
@@ -1367,10 +3023,82 @@
       <c r="K23">
         <v>1670</v>
       </c>
+      <c r="L23">
+        <v>5460</v>
+      </c>
+      <c r="M23">
+        <v>4919000</v>
+      </c>
+      <c r="N23">
+        <v>3345000</v>
+      </c>
+      <c r="O23">
+        <v>61.3</v>
+      </c>
+      <c r="P23">
+        <v>2.2</v>
+      </c>
+      <c r="Q23">
+        <v>68</v>
+      </c>
+      <c r="R23">
+        <v>2.2</v>
+      </c>
+      <c r="S23">
+        <v>2731000</v>
+      </c>
+      <c r="T23">
+        <v>50</v>
+      </c>
+      <c r="U23">
+        <v>2.2</v>
+      </c>
+      <c r="V23">
+        <v>55.5</v>
+      </c>
+      <c r="W23">
+        <v>2.3</v>
+      </c>
+      <c r="X23">
+        <v>5170</v>
+      </c>
+      <c r="Y23">
+        <v>4774000</v>
+      </c>
+      <c r="Z23">
+        <v>3759000</v>
+      </c>
+      <c r="AA23">
+        <v>72.7</v>
+      </c>
+      <c r="AB23">
+        <v>1.8</v>
+      </c>
+      <c r="AC23">
+        <v>78.7</v>
+      </c>
+      <c r="AD23">
+        <v>1.8</v>
+      </c>
+      <c r="AE23">
+        <v>3382000</v>
+      </c>
+      <c r="AF23">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="AG23">
+        <v>2</v>
+      </c>
+      <c r="AH23">
+        <v>70.8</v>
+      </c>
+      <c r="AI23">
+        <v>2</v>
+      </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:35">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B24">
         <v>0.4336012865605604</v>
@@ -1402,10 +3130,82 @@
       <c r="K24">
         <v>26934</v>
       </c>
+      <c r="L24">
+        <v>7657</v>
+      </c>
+      <c r="M24">
+        <v>7430000</v>
+      </c>
+      <c r="N24">
+        <v>5453000</v>
+      </c>
+      <c r="O24">
+        <v>71.2</v>
+      </c>
+      <c r="P24">
+        <v>1.7</v>
+      </c>
+      <c r="Q24">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="R24">
+        <v>1.7</v>
+      </c>
+      <c r="S24">
+        <v>4418000</v>
+      </c>
+      <c r="T24">
+        <v>57.7</v>
+      </c>
+      <c r="U24">
+        <v>1.9</v>
+      </c>
+      <c r="V24">
+        <v>59.5</v>
+      </c>
+      <c r="W24">
+        <v>1.9</v>
+      </c>
+      <c r="X24">
+        <v>7496</v>
+      </c>
+      <c r="Y24">
+        <v>7228000</v>
+      </c>
+      <c r="Z24">
+        <v>5620000</v>
+      </c>
+      <c r="AA24">
+        <v>75</v>
+      </c>
+      <c r="AB24">
+        <v>1.5</v>
+      </c>
+      <c r="AC24">
+        <v>77.8</v>
+      </c>
+      <c r="AD24">
+        <v>1.5</v>
+      </c>
+      <c r="AE24">
+        <v>4832000</v>
+      </c>
+      <c r="AF24">
+        <v>64.5</v>
+      </c>
+      <c r="AG24">
+        <v>1.7</v>
+      </c>
+      <c r="AH24">
+        <v>66.8</v>
+      </c>
+      <c r="AI24">
+        <v>1.7</v>
+      </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:35">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B25">
         <v>0.4454040370754654</v>
@@ -1437,10 +3237,82 @@
       <c r="K25">
         <v>46080</v>
       </c>
+      <c r="L25">
+        <v>4238</v>
+      </c>
+      <c r="M25">
+        <v>4006000</v>
+      </c>
+      <c r="N25">
+        <v>3000000</v>
+      </c>
+      <c r="O25">
+        <v>70.8</v>
+      </c>
+      <c r="P25">
+        <v>2.3</v>
+      </c>
+      <c r="Q25">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="R25">
+        <v>2.3</v>
+      </c>
+      <c r="S25">
+        <v>2523000</v>
+      </c>
+      <c r="T25">
+        <v>59.5</v>
+      </c>
+      <c r="U25">
+        <v>2.5</v>
+      </c>
+      <c r="V25">
+        <v>63</v>
+      </c>
+      <c r="W25">
+        <v>2.5</v>
+      </c>
+      <c r="X25">
+        <v>4055</v>
+      </c>
+      <c r="Y25">
+        <v>3903000</v>
+      </c>
+      <c r="Z25">
+        <v>3085000</v>
+      </c>
+      <c r="AA25">
+        <v>76.09999999999999</v>
+      </c>
+      <c r="AB25">
+        <v>2</v>
+      </c>
+      <c r="AC25">
+        <v>79</v>
+      </c>
+      <c r="AD25">
+        <v>1.9</v>
+      </c>
+      <c r="AE25">
+        <v>2859000</v>
+      </c>
+      <c r="AF25">
+        <v>70.5</v>
+      </c>
+      <c r="AG25">
+        <v>2.1</v>
+      </c>
+      <c r="AH25">
+        <v>73.2</v>
+      </c>
+      <c r="AI25">
+        <v>2.1</v>
+      </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:35">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="B26">
         <v>0.5925505236628795</v>
@@ -1472,10 +3344,82 @@
       <c r="K26">
         <v>20474</v>
       </c>
+      <c r="L26">
+        <v>2194</v>
+      </c>
+      <c r="M26">
+        <v>2178000</v>
+      </c>
+      <c r="N26">
+        <v>1599000</v>
+      </c>
+      <c r="O26">
+        <v>72.90000000000001</v>
+      </c>
+      <c r="P26">
+        <v>2.5</v>
+      </c>
+      <c r="Q26">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="R26">
+        <v>2.5</v>
+      </c>
+      <c r="S26">
+        <v>1180000</v>
+      </c>
+      <c r="T26">
+        <v>53.8</v>
+      </c>
+      <c r="U26">
+        <v>2.8</v>
+      </c>
+      <c r="V26">
+        <v>54.2</v>
+      </c>
+      <c r="W26">
+        <v>2.8</v>
+      </c>
+      <c r="X26">
+        <v>2166</v>
+      </c>
+      <c r="Y26">
+        <v>2130000</v>
+      </c>
+      <c r="Z26">
+        <v>1794000</v>
+      </c>
+      <c r="AA26">
+        <v>82.8</v>
+      </c>
+      <c r="AB26">
+        <v>2</v>
+      </c>
+      <c r="AC26">
+        <v>84.2</v>
+      </c>
+      <c r="AD26">
+        <v>1.9</v>
+      </c>
+      <c r="AE26">
+        <v>1588000</v>
+      </c>
+      <c r="AF26">
+        <v>73.3</v>
+      </c>
+      <c r="AG26">
+        <v>2.3</v>
+      </c>
+      <c r="AH26">
+        <v>74.5</v>
+      </c>
+      <c r="AI26">
+        <v>2.3</v>
+      </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:35">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="B27">
         <v>0.46202628237611</v>
@@ -1507,10 +3451,82 @@
       <c r="K27">
         <v>57682</v>
       </c>
+      <c r="L27">
+        <v>4676</v>
+      </c>
+      <c r="M27">
+        <v>4564000</v>
+      </c>
+      <c r="N27">
+        <v>3299000</v>
+      </c>
+      <c r="O27">
+        <v>70.59999999999999</v>
+      </c>
+      <c r="P27">
+        <v>2.2</v>
+      </c>
+      <c r="Q27">
+        <v>72.3</v>
+      </c>
+      <c r="R27">
+        <v>2.2</v>
+      </c>
+      <c r="S27">
+        <v>2509000</v>
+      </c>
+      <c r="T27">
+        <v>53.7</v>
+      </c>
+      <c r="U27">
+        <v>2.4</v>
+      </c>
+      <c r="V27">
+        <v>55</v>
+      </c>
+      <c r="W27">
+        <v>2.5</v>
+      </c>
+      <c r="X27">
+        <v>4521</v>
+      </c>
+      <c r="Y27">
+        <v>4409000</v>
+      </c>
+      <c r="Z27">
+        <v>3384000</v>
+      </c>
+      <c r="AA27">
+        <v>74.8</v>
+      </c>
+      <c r="AB27">
+        <v>1.9</v>
+      </c>
+      <c r="AC27">
+        <v>76.7</v>
+      </c>
+      <c r="AD27">
+        <v>1.9</v>
+      </c>
+      <c r="AE27">
+        <v>2818000</v>
+      </c>
+      <c r="AF27">
+        <v>62.3</v>
+      </c>
+      <c r="AG27">
+        <v>2.2</v>
+      </c>
+      <c r="AH27">
+        <v>63.9</v>
+      </c>
+      <c r="AI27">
+        <v>2.2</v>
+      </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:35">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="B28">
         <v>0.4859271009150489</v>
@@ -1542,10 +3558,82 @@
       <c r="K28">
         <v>11685</v>
       </c>
+      <c r="L28">
+        <v>822</v>
+      </c>
+      <c r="M28">
+        <v>812000</v>
+      </c>
+      <c r="N28">
+        <v>579000</v>
+      </c>
+      <c r="O28">
+        <v>70.40000000000001</v>
+      </c>
+      <c r="P28">
+        <v>2.3</v>
+      </c>
+      <c r="Q28">
+        <v>71.3</v>
+      </c>
+      <c r="R28">
+        <v>2.3</v>
+      </c>
+      <c r="S28">
+        <v>518000</v>
+      </c>
+      <c r="T28">
+        <v>63</v>
+      </c>
+      <c r="U28">
+        <v>2.4</v>
+      </c>
+      <c r="V28">
+        <v>63.8</v>
+      </c>
+      <c r="W28">
+        <v>2.4</v>
+      </c>
+      <c r="X28">
+        <v>768</v>
+      </c>
+      <c r="Y28">
+        <v>754000</v>
+      </c>
+      <c r="Z28">
+        <v>553000</v>
+      </c>
+      <c r="AA28">
+        <v>72</v>
+      </c>
+      <c r="AB28">
+        <v>2.3</v>
+      </c>
+      <c r="AC28">
+        <v>73.3</v>
+      </c>
+      <c r="AD28">
+        <v>2.3</v>
+      </c>
+      <c r="AE28">
+        <v>495000</v>
+      </c>
+      <c r="AF28">
+        <v>64.5</v>
+      </c>
+      <c r="AG28">
+        <v>2.4</v>
+      </c>
+      <c r="AH28">
+        <v>65.7</v>
+      </c>
+      <c r="AI28">
+        <v>2.4</v>
+      </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:35">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="B29">
         <v>0.564037131587158</v>
@@ -1577,10 +3665,82 @@
       <c r="K29">
         <v>35194</v>
       </c>
+      <c r="L29">
+        <v>1428</v>
+      </c>
+      <c r="M29">
+        <v>1332000</v>
+      </c>
+      <c r="N29">
+        <v>883000</v>
+      </c>
+      <c r="O29">
+        <v>61.9</v>
+      </c>
+      <c r="P29">
+        <v>2.8</v>
+      </c>
+      <c r="Q29">
+        <v>66.3</v>
+      </c>
+      <c r="R29">
+        <v>2.8</v>
+      </c>
+      <c r="S29">
+        <v>676000</v>
+      </c>
+      <c r="T29">
+        <v>47.3</v>
+      </c>
+      <c r="U29">
+        <v>2.9</v>
+      </c>
+      <c r="V29">
+        <v>50.8</v>
+      </c>
+      <c r="W29">
+        <v>3</v>
+      </c>
+      <c r="X29">
+        <v>1371</v>
+      </c>
+      <c r="Y29">
+        <v>1296000</v>
+      </c>
+      <c r="Z29">
+        <v>901000</v>
+      </c>
+      <c r="AA29">
+        <v>65.7</v>
+      </c>
+      <c r="AB29">
+        <v>2.5</v>
+      </c>
+      <c r="AC29">
+        <v>69.5</v>
+      </c>
+      <c r="AD29">
+        <v>2.5</v>
+      </c>
+      <c r="AE29">
+        <v>798000</v>
+      </c>
+      <c r="AF29">
+        <v>58.2</v>
+      </c>
+      <c r="AG29">
+        <v>2.6</v>
+      </c>
+      <c r="AH29">
+        <v>61.6</v>
+      </c>
+      <c r="AI29">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:35">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B30">
         <v>0.723674365163597</v>
@@ -1612,10 +3772,82 @@
       <c r="K30">
         <v>2784</v>
       </c>
+      <c r="L30">
+        <v>2324</v>
+      </c>
+      <c r="M30">
+        <v>2067000</v>
+      </c>
+      <c r="N30">
+        <v>1277000</v>
+      </c>
+      <c r="O30">
+        <v>55</v>
+      </c>
+      <c r="P30">
+        <v>2.7</v>
+      </c>
+      <c r="Q30">
+        <v>61.8</v>
+      </c>
+      <c r="R30">
+        <v>2.8</v>
+      </c>
+      <c r="S30">
+        <v>1006000</v>
+      </c>
+      <c r="T30">
+        <v>43.3</v>
+      </c>
+      <c r="U30">
+        <v>2.7</v>
+      </c>
+      <c r="V30">
+        <v>48.7</v>
+      </c>
+      <c r="W30">
+        <v>2.9</v>
+      </c>
+      <c r="X30">
+        <v>2039</v>
+      </c>
+      <c r="Y30">
+        <v>1808000</v>
+      </c>
+      <c r="Z30">
+        <v>1176000</v>
+      </c>
+      <c r="AA30">
+        <v>57.7</v>
+      </c>
+      <c r="AB30">
+        <v>2.5</v>
+      </c>
+      <c r="AC30">
+        <v>65</v>
+      </c>
+      <c r="AD30">
+        <v>2.6</v>
+      </c>
+      <c r="AE30">
+        <v>1048000</v>
+      </c>
+      <c r="AF30">
+        <v>51.4</v>
+      </c>
+      <c r="AG30">
+        <v>2.5</v>
+      </c>
+      <c r="AH30">
+        <v>57.9</v>
+      </c>
+      <c r="AI30">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:35">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B31">
         <v>0.4600200283283563</v>
@@ -1647,10 +3879,82 @@
       <c r="K31">
         <v>2114</v>
       </c>
+      <c r="L31">
+        <v>1080</v>
+      </c>
+      <c r="M31">
+        <v>1025000</v>
+      </c>
+      <c r="N31">
+        <v>726000</v>
+      </c>
+      <c r="O31">
+        <v>67.2</v>
+      </c>
+      <c r="P31">
+        <v>2.6</v>
+      </c>
+      <c r="Q31">
+        <v>70.8</v>
+      </c>
+      <c r="R31">
+        <v>2.6</v>
+      </c>
+      <c r="S31">
+        <v>576000</v>
+      </c>
+      <c r="T31">
+        <v>53.3</v>
+      </c>
+      <c r="U31">
+        <v>2.8</v>
+      </c>
+      <c r="V31">
+        <v>56.2</v>
+      </c>
+      <c r="W31">
+        <v>2.8</v>
+      </c>
+      <c r="X31">
+        <v>1028</v>
+      </c>
+      <c r="Y31">
+        <v>991000</v>
+      </c>
+      <c r="Z31">
+        <v>752000</v>
+      </c>
+      <c r="AA31">
+        <v>73.09999999999999</v>
+      </c>
+      <c r="AB31">
+        <v>2.4</v>
+      </c>
+      <c r="AC31">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="AD31">
+        <v>2.3</v>
+      </c>
+      <c r="AE31">
+        <v>688000</v>
+      </c>
+      <c r="AF31">
+        <v>66.90000000000001</v>
+      </c>
+      <c r="AG31">
+        <v>2.5</v>
+      </c>
+      <c r="AH31">
+        <v>69.40000000000001</v>
+      </c>
+      <c r="AI31">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:35">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="B32">
         <v>0.09961453566527755</v>
@@ -1682,10 +3986,82 @@
       <c r="K32">
         <v>1261</v>
       </c>
+      <c r="L32">
+        <v>7009</v>
+      </c>
+      <c r="M32">
+        <v>6267000</v>
+      </c>
+      <c r="N32">
+        <v>4297000</v>
+      </c>
+      <c r="O32">
+        <v>61.3</v>
+      </c>
+      <c r="P32">
+        <v>1.9</v>
+      </c>
+      <c r="Q32">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="R32">
+        <v>1.9</v>
+      </c>
+      <c r="S32">
+        <v>3384000</v>
+      </c>
+      <c r="T32">
+        <v>48.3</v>
+      </c>
+      <c r="U32">
+        <v>2</v>
+      </c>
+      <c r="V32">
+        <v>54</v>
+      </c>
+      <c r="W32">
+        <v>2.1</v>
+      </c>
+      <c r="X32">
+        <v>6730</v>
+      </c>
+      <c r="Y32">
+        <v>5929000</v>
+      </c>
+      <c r="Z32">
+        <v>4326000</v>
+      </c>
+      <c r="AA32">
+        <v>64.3</v>
+      </c>
+      <c r="AB32">
+        <v>1.8</v>
+      </c>
+      <c r="AC32">
+        <v>73</v>
+      </c>
+      <c r="AD32">
+        <v>1.7</v>
+      </c>
+      <c r="AE32">
+        <v>3670000</v>
+      </c>
+      <c r="AF32">
+        <v>54.5</v>
+      </c>
+      <c r="AG32">
+        <v>1.8</v>
+      </c>
+      <c r="AH32">
+        <v>61.9</v>
+      </c>
+      <c r="AI32">
+        <v>1.9</v>
+      </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:35">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="B33">
         <v>0.7457235005223746</v>
@@ -1717,10 +4093,82 @@
       <c r="K33">
         <v>18477</v>
       </c>
+      <c r="L33">
+        <v>1576</v>
+      </c>
+      <c r="M33">
+        <v>1485000</v>
+      </c>
+      <c r="N33">
+        <v>916000</v>
+      </c>
+      <c r="O33">
+        <v>58.1</v>
+      </c>
+      <c r="P33">
+        <v>2.5</v>
+      </c>
+      <c r="Q33">
+        <v>61.7</v>
+      </c>
+      <c r="R33">
+        <v>2.6</v>
+      </c>
+      <c r="S33">
+        <v>715000</v>
+      </c>
+      <c r="T33">
+        <v>45.3</v>
+      </c>
+      <c r="U33">
+        <v>2.6</v>
+      </c>
+      <c r="V33">
+        <v>48.1</v>
+      </c>
+      <c r="W33">
+        <v>2.6</v>
+      </c>
+      <c r="X33">
+        <v>1553</v>
+      </c>
+      <c r="Y33">
+        <v>1426000</v>
+      </c>
+      <c r="Z33">
+        <v>978000</v>
+      </c>
+      <c r="AA33">
+        <v>63</v>
+      </c>
+      <c r="AB33">
+        <v>2.5</v>
+      </c>
+      <c r="AC33">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="AD33">
+        <v>2.5</v>
+      </c>
+      <c r="AE33">
+        <v>878000</v>
+      </c>
+      <c r="AF33">
+        <v>56.5</v>
+      </c>
+      <c r="AG33">
+        <v>2.5</v>
+      </c>
+      <c r="AH33">
+        <v>61.6</v>
+      </c>
+      <c r="AI33">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:35">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B34">
         <v>0.6309524493519199</v>
@@ -1752,10 +4200,82 @@
       <c r="K34">
         <v>20640</v>
       </c>
+      <c r="L34">
+        <v>15478</v>
+      </c>
+      <c r="M34">
+        <v>13684000</v>
+      </c>
+      <c r="N34">
+        <v>8553000</v>
+      </c>
+      <c r="O34">
+        <v>55.3</v>
+      </c>
+      <c r="P34">
+        <v>1.3</v>
+      </c>
+      <c r="Q34">
+        <v>62.5</v>
+      </c>
+      <c r="R34">
+        <v>1.4</v>
+      </c>
+      <c r="S34">
+        <v>6775000</v>
+      </c>
+      <c r="T34">
+        <v>43.8</v>
+      </c>
+      <c r="U34">
+        <v>1.3</v>
+      </c>
+      <c r="V34">
+        <v>49.5</v>
+      </c>
+      <c r="W34">
+        <v>1.4</v>
+      </c>
+      <c r="X34">
+        <v>15066</v>
+      </c>
+      <c r="Y34">
+        <v>13082000</v>
+      </c>
+      <c r="Z34">
+        <v>8887000</v>
+      </c>
+      <c r="AA34">
+        <v>59</v>
+      </c>
+      <c r="AB34">
+        <v>1.2</v>
+      </c>
+      <c r="AC34">
+        <v>67.90000000000001</v>
+      </c>
+      <c r="AD34">
+        <v>1.2</v>
+      </c>
+      <c r="AE34">
+        <v>7675000</v>
+      </c>
+      <c r="AF34">
+        <v>50.9</v>
+      </c>
+      <c r="AG34">
+        <v>1.2</v>
+      </c>
+      <c r="AH34">
+        <v>58.7</v>
+      </c>
+      <c r="AI34">
+        <v>1.3</v>
+      </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:35">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="B35">
         <v>0.6812640238286974</v>
@@ -1787,10 +4307,82 @@
       <c r="K35">
         <v>30358</v>
       </c>
+      <c r="L35">
+        <v>7911</v>
+      </c>
+      <c r="M35">
+        <v>7444000</v>
+      </c>
+      <c r="N35">
+        <v>5160000</v>
+      </c>
+      <c r="O35">
+        <v>65.2</v>
+      </c>
+      <c r="P35">
+        <v>1.8</v>
+      </c>
+      <c r="Q35">
+        <v>69.3</v>
+      </c>
+      <c r="R35">
+        <v>1.8</v>
+      </c>
+      <c r="S35">
+        <v>3899000</v>
+      </c>
+      <c r="T35">
+        <v>49.3</v>
+      </c>
+      <c r="U35">
+        <v>1.9</v>
+      </c>
+      <c r="V35">
+        <v>52.4</v>
+      </c>
+      <c r="W35">
+        <v>1.9</v>
+      </c>
+      <c r="X35">
+        <v>7265</v>
+      </c>
+      <c r="Y35">
+        <v>6712000</v>
+      </c>
+      <c r="Z35">
+        <v>5295000</v>
+      </c>
+      <c r="AA35">
+        <v>72.90000000000001</v>
+      </c>
+      <c r="AB35">
+        <v>1.6</v>
+      </c>
+      <c r="AC35">
+        <v>78.90000000000001</v>
+      </c>
+      <c r="AD35">
+        <v>1.5</v>
+      </c>
+      <c r="AE35">
+        <v>4624000</v>
+      </c>
+      <c r="AF35">
+        <v>63.7</v>
+      </c>
+      <c r="AG35">
+        <v>1.7</v>
+      </c>
+      <c r="AH35">
+        <v>68.90000000000001</v>
+      </c>
+      <c r="AI35">
+        <v>1.7</v>
+      </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:35">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="B36">
         <v>0.1584721397732975</v>
@@ -1822,10 +4414,82 @@
       <c r="K36">
         <v>9334</v>
       </c>
+      <c r="L36">
+        <v>560</v>
+      </c>
+      <c r="M36">
+        <v>541000</v>
+      </c>
+      <c r="N36">
+        <v>397000</v>
+      </c>
+      <c r="O36">
+        <v>70.90000000000001</v>
+      </c>
+      <c r="P36">
+        <v>2.5</v>
+      </c>
+      <c r="Q36">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="R36">
+        <v>2.5</v>
+      </c>
+      <c r="S36">
+        <v>335000</v>
+      </c>
+      <c r="T36">
+        <v>59.8</v>
+      </c>
+      <c r="U36">
+        <v>2.7</v>
+      </c>
+      <c r="V36">
+        <v>61.9</v>
+      </c>
+      <c r="W36">
+        <v>2.7</v>
+      </c>
+      <c r="X36">
+        <v>528</v>
+      </c>
+      <c r="Y36">
+        <v>514000</v>
+      </c>
+      <c r="Z36">
+        <v>383000</v>
+      </c>
+      <c r="AA36">
+        <v>72.5</v>
+      </c>
+      <c r="AB36">
+        <v>2.3</v>
+      </c>
+      <c r="AC36">
+        <v>74.5</v>
+      </c>
+      <c r="AD36">
+        <v>2.3</v>
+      </c>
+      <c r="AE36">
+        <v>328000</v>
+      </c>
+      <c r="AF36">
+        <v>62.2</v>
+      </c>
+      <c r="AG36">
+        <v>2.5</v>
+      </c>
+      <c r="AH36">
+        <v>63.9</v>
+      </c>
+      <c r="AI36">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:35">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B37">
         <v>0.4073767938647649</v>
@@ -1857,10 +4521,82 @@
       <c r="K37">
         <v>40954</v>
       </c>
+      <c r="L37">
+        <v>8873</v>
+      </c>
+      <c r="M37">
+        <v>8640000</v>
+      </c>
+      <c r="N37">
+        <v>6062000</v>
+      </c>
+      <c r="O37">
+        <v>68.3</v>
+      </c>
+      <c r="P37">
+        <v>1.6</v>
+      </c>
+      <c r="Q37">
+        <v>70.2</v>
+      </c>
+      <c r="R37">
+        <v>1.6</v>
+      </c>
+      <c r="S37">
+        <v>4538000</v>
+      </c>
+      <c r="T37">
+        <v>51.1</v>
+      </c>
+      <c r="U37">
+        <v>1.8</v>
+      </c>
+      <c r="V37">
+        <v>52.5</v>
+      </c>
+      <c r="W37">
+        <v>1.8</v>
+      </c>
+      <c r="X37">
+        <v>8750</v>
+      </c>
+      <c r="Y37">
+        <v>8550000</v>
+      </c>
+      <c r="Z37">
+        <v>6076000</v>
+      </c>
+      <c r="AA37">
+        <v>69.40000000000001</v>
+      </c>
+      <c r="AB37">
+        <v>1.5</v>
+      </c>
+      <c r="AC37">
+        <v>71.09999999999999</v>
+      </c>
+      <c r="AD37">
+        <v>1.5</v>
+      </c>
+      <c r="AE37">
+        <v>5395000</v>
+      </c>
+      <c r="AF37">
+        <v>61.7</v>
+      </c>
+      <c r="AG37">
+        <v>1.6</v>
+      </c>
+      <c r="AH37">
+        <v>63.1</v>
+      </c>
+      <c r="AI37">
+        <v>1.6</v>
+      </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:35">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B38">
         <v>0.7930828453257812</v>
@@ -1892,10 +4628,82 @@
       <c r="K38">
         <v>57871</v>
       </c>
+      <c r="L38">
+        <v>2868</v>
+      </c>
+      <c r="M38">
+        <v>2732000</v>
+      </c>
+      <c r="N38">
+        <v>1777000</v>
+      </c>
+      <c r="O38">
+        <v>62</v>
+      </c>
+      <c r="P38">
+        <v>2.9</v>
+      </c>
+      <c r="Q38">
+        <v>65.09999999999999</v>
+      </c>
+      <c r="R38">
+        <v>2.9</v>
+      </c>
+      <c r="S38">
+        <v>1350000</v>
+      </c>
+      <c r="T38">
+        <v>47.1</v>
+      </c>
+      <c r="U38">
+        <v>3</v>
+      </c>
+      <c r="V38">
+        <v>49.4</v>
+      </c>
+      <c r="W38">
+        <v>3</v>
+      </c>
+      <c r="X38">
+        <v>2808</v>
+      </c>
+      <c r="Y38">
+        <v>2733000</v>
+      </c>
+      <c r="Z38">
+        <v>1806000</v>
+      </c>
+      <c r="AA38">
+        <v>64.3</v>
+      </c>
+      <c r="AB38">
+        <v>2.5</v>
+      </c>
+      <c r="AC38">
+        <v>66.09999999999999</v>
+      </c>
+      <c r="AD38">
+        <v>2.5</v>
+      </c>
+      <c r="AE38">
+        <v>1431000</v>
+      </c>
+      <c r="AF38">
+        <v>51</v>
+      </c>
+      <c r="AG38">
+        <v>2.6</v>
+      </c>
+      <c r="AH38">
+        <v>52.4</v>
+      </c>
+      <c r="AI38">
+        <v>2.6</v>
+      </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:35">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="B39">
         <v>0.3149294544387963</v>
@@ -1927,10 +4735,82 @@
       <c r="K39">
         <v>11830</v>
       </c>
+      <c r="L39">
+        <v>3293</v>
+      </c>
+      <c r="M39">
+        <v>3138000</v>
+      </c>
+      <c r="N39">
+        <v>2274000</v>
+      </c>
+      <c r="O39">
+        <v>69.09999999999999</v>
+      </c>
+      <c r="P39">
+        <v>2.6</v>
+      </c>
+      <c r="Q39">
+        <v>72.5</v>
+      </c>
+      <c r="R39">
+        <v>2.5</v>
+      </c>
+      <c r="S39">
+        <v>1918000</v>
+      </c>
+      <c r="T39">
+        <v>58.2</v>
+      </c>
+      <c r="U39">
+        <v>2.7</v>
+      </c>
+      <c r="V39">
+        <v>61.1</v>
+      </c>
+      <c r="W39">
+        <v>2.8</v>
+      </c>
+      <c r="X39">
+        <v>2998</v>
+      </c>
+      <c r="Y39">
+        <v>2806000</v>
+      </c>
+      <c r="Z39">
+        <v>2086000</v>
+      </c>
+      <c r="AA39">
+        <v>69.59999999999999</v>
+      </c>
+      <c r="AB39">
+        <v>2.4</v>
+      </c>
+      <c r="AC39">
+        <v>74.3</v>
+      </c>
+      <c r="AD39">
+        <v>2.3</v>
+      </c>
+      <c r="AE39">
+        <v>1897000</v>
+      </c>
+      <c r="AF39">
+        <v>63.3</v>
+      </c>
+      <c r="AG39">
+        <v>2.5</v>
+      </c>
+      <c r="AH39">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="AI39">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:35">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B40">
         <v>0.6347643611259925</v>
@@ -1962,10 +4842,82 @@
       <c r="K40">
         <v>38727</v>
       </c>
+      <c r="L40">
+        <v>9928</v>
+      </c>
+      <c r="M40">
+        <v>9475000</v>
+      </c>
+      <c r="N40">
+        <v>6469000</v>
+      </c>
+      <c r="O40">
+        <v>65.2</v>
+      </c>
+      <c r="P40">
+        <v>1.6</v>
+      </c>
+      <c r="Q40">
+        <v>68.3</v>
+      </c>
+      <c r="R40">
+        <v>1.6</v>
+      </c>
+      <c r="S40">
+        <v>5173000</v>
+      </c>
+      <c r="T40">
+        <v>52.1</v>
+      </c>
+      <c r="U40">
+        <v>1.7</v>
+      </c>
+      <c r="V40">
+        <v>54.6</v>
+      </c>
+      <c r="W40">
+        <v>1.7</v>
+      </c>
+      <c r="X40">
+        <v>9847</v>
+      </c>
+      <c r="Y40">
+        <v>9452000</v>
+      </c>
+      <c r="Z40">
+        <v>6795000</v>
+      </c>
+      <c r="AA40">
+        <v>69</v>
+      </c>
+      <c r="AB40">
+        <v>1.4</v>
+      </c>
+      <c r="AC40">
+        <v>71.90000000000001</v>
+      </c>
+      <c r="AD40">
+        <v>1.4</v>
+      </c>
+      <c r="AE40">
+        <v>5824000</v>
+      </c>
+      <c r="AF40">
+        <v>59.1</v>
+      </c>
+      <c r="AG40">
+        <v>1.5</v>
+      </c>
+      <c r="AH40">
+        <v>61.6</v>
+      </c>
+      <c r="AI40">
+        <v>1.5</v>
+      </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:35">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B41">
         <v>0.3794571656413762</v>
@@ -1997,10 +4949,82 @@
       <c r="K41">
         <v>275</v>
       </c>
+      <c r="L41">
+        <v>828</v>
+      </c>
+      <c r="M41">
+        <v>782000</v>
+      </c>
+      <c r="N41">
+        <v>532000</v>
+      </c>
+      <c r="O41">
+        <v>64.2</v>
+      </c>
+      <c r="P41">
+        <v>2.7</v>
+      </c>
+      <c r="Q41">
+        <v>68</v>
+      </c>
+      <c r="R41">
+        <v>2.7</v>
+      </c>
+      <c r="S41">
+        <v>403000</v>
+      </c>
+      <c r="T41">
+        <v>48.7</v>
+      </c>
+      <c r="U41">
+        <v>2.8</v>
+      </c>
+      <c r="V41">
+        <v>51.6</v>
+      </c>
+      <c r="W41">
+        <v>2.9</v>
+      </c>
+      <c r="X41">
+        <v>817</v>
+      </c>
+      <c r="Y41">
+        <v>751000</v>
+      </c>
+      <c r="Z41">
+        <v>552000</v>
+      </c>
+      <c r="AA41">
+        <v>67.5</v>
+      </c>
+      <c r="AB41">
+        <v>2.5</v>
+      </c>
+      <c r="AC41">
+        <v>73.5</v>
+      </c>
+      <c r="AD41">
+        <v>2.5</v>
+      </c>
+      <c r="AE41">
+        <v>469000</v>
+      </c>
+      <c r="AF41">
+        <v>57.4</v>
+      </c>
+      <c r="AG41">
+        <v>2.7</v>
+      </c>
+      <c r="AH41">
+        <v>62.5</v>
+      </c>
+      <c r="AI41">
+        <v>2.7</v>
+      </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:35">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B42">
         <v>0.5744615138239096</v>
@@ -2032,10 +5056,82 @@
       <c r="K42">
         <v>14015</v>
       </c>
+      <c r="L42">
+        <v>3914</v>
+      </c>
+      <c r="M42">
+        <v>3769000</v>
+      </c>
+      <c r="N42">
+        <v>2430000</v>
+      </c>
+      <c r="O42">
+        <v>62.1</v>
+      </c>
+      <c r="P42">
+        <v>2.5</v>
+      </c>
+      <c r="Q42">
+        <v>64.5</v>
+      </c>
+      <c r="R42">
+        <v>2.5</v>
+      </c>
+      <c r="S42">
+        <v>1836000</v>
+      </c>
+      <c r="T42">
+        <v>46.9</v>
+      </c>
+      <c r="U42">
+        <v>2.6</v>
+      </c>
+      <c r="V42">
+        <v>48.7</v>
+      </c>
+      <c r="W42">
+        <v>2.7</v>
+      </c>
+      <c r="X42">
+        <v>3516</v>
+      </c>
+      <c r="Y42">
+        <v>3380000</v>
+      </c>
+      <c r="Z42">
+        <v>2479000</v>
+      </c>
+      <c r="AA42">
+        <v>70.5</v>
+      </c>
+      <c r="AB42">
+        <v>2.3</v>
+      </c>
+      <c r="AC42">
+        <v>73.3</v>
+      </c>
+      <c r="AD42">
+        <v>2.3</v>
+      </c>
+      <c r="AE42">
+        <v>2187000</v>
+      </c>
+      <c r="AF42">
+        <v>62.2</v>
+      </c>
+      <c r="AG42">
+        <v>2.4</v>
+      </c>
+      <c r="AH42">
+        <v>64.7</v>
+      </c>
+      <c r="AI42">
+        <v>2.4</v>
+      </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:35">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B43">
         <v>0.4388594775675316</v>
@@ -2067,10 +5163,82 @@
       <c r="K43">
         <v>19161</v>
       </c>
+      <c r="L43">
+        <v>648</v>
+      </c>
+      <c r="M43">
+        <v>637000</v>
+      </c>
+      <c r="N43">
+        <v>429000</v>
+      </c>
+      <c r="O43">
+        <v>66.2</v>
+      </c>
+      <c r="P43">
+        <v>2.7</v>
+      </c>
+      <c r="Q43">
+        <v>67.3</v>
+      </c>
+      <c r="R43">
+        <v>2.7</v>
+      </c>
+      <c r="S43">
+        <v>331000</v>
+      </c>
+      <c r="T43">
+        <v>51</v>
+      </c>
+      <c r="U43">
+        <v>2.9</v>
+      </c>
+      <c r="V43">
+        <v>51.9</v>
+      </c>
+      <c r="W43">
+        <v>2.9</v>
+      </c>
+      <c r="X43">
+        <v>616</v>
+      </c>
+      <c r="Y43">
+        <v>607000</v>
+      </c>
+      <c r="Z43">
+        <v>454000</v>
+      </c>
+      <c r="AA43">
+        <v>73.7</v>
+      </c>
+      <c r="AB43">
+        <v>2.1</v>
+      </c>
+      <c r="AC43">
+        <v>74.8</v>
+      </c>
+      <c r="AD43">
+        <v>2.1</v>
+      </c>
+      <c r="AE43">
+        <v>370000</v>
+      </c>
+      <c r="AF43">
+        <v>60.1</v>
+      </c>
+      <c r="AG43">
+        <v>2.4</v>
+      </c>
+      <c r="AH43">
+        <v>61</v>
+      </c>
+      <c r="AI43">
+        <v>2.4</v>
+      </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:35">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="B44">
         <v>0.4006291154683535</v>
@@ -2102,10 +5270,82 @@
       <c r="K44">
         <v>36319</v>
       </c>
+      <c r="L44">
+        <v>5202</v>
+      </c>
+      <c r="M44">
+        <v>5016000</v>
+      </c>
+      <c r="N44">
+        <v>3183000</v>
+      </c>
+      <c r="O44">
+        <v>61.2</v>
+      </c>
+      <c r="P44">
+        <v>2.2</v>
+      </c>
+      <c r="Q44">
+        <v>63.5</v>
+      </c>
+      <c r="R44">
+        <v>2.2</v>
+      </c>
+      <c r="S44">
+        <v>2487000</v>
+      </c>
+      <c r="T44">
+        <v>47.8</v>
+      </c>
+      <c r="U44">
+        <v>2.3</v>
+      </c>
+      <c r="V44">
+        <v>49.6</v>
+      </c>
+      <c r="W44">
+        <v>2.3</v>
+      </c>
+      <c r="X44">
+        <v>4849</v>
+      </c>
+      <c r="Y44">
+        <v>4678000</v>
+      </c>
+      <c r="Z44">
+        <v>3210000</v>
+      </c>
+      <c r="AA44">
+        <v>66.2</v>
+      </c>
+      <c r="AB44">
+        <v>2</v>
+      </c>
+      <c r="AC44">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="AD44">
+        <v>2</v>
+      </c>
+      <c r="AE44">
+        <v>2606000</v>
+      </c>
+      <c r="AF44">
+        <v>53.7</v>
+      </c>
+      <c r="AG44">
+        <v>2.1</v>
+      </c>
+      <c r="AH44">
+        <v>55.7</v>
+      </c>
+      <c r="AI44">
+        <v>2.2</v>
+      </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:35">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B45">
         <v>0.6490816851955948</v>
@@ -2137,10 +5377,82 @@
       <c r="K45">
         <v>169213</v>
       </c>
+      <c r="L45">
+        <v>21064</v>
+      </c>
+      <c r="M45">
+        <v>18374000</v>
+      </c>
+      <c r="N45">
+        <v>11634000</v>
+      </c>
+      <c r="O45">
+        <v>55.2</v>
+      </c>
+      <c r="P45">
+        <v>1.1</v>
+      </c>
+      <c r="Q45">
+        <v>63.3</v>
+      </c>
+      <c r="R45">
+        <v>1.2</v>
+      </c>
+      <c r="S45">
+        <v>8886000</v>
+      </c>
+      <c r="T45">
+        <v>42.2</v>
+      </c>
+      <c r="U45">
+        <v>1.1</v>
+      </c>
+      <c r="V45">
+        <v>48.4</v>
+      </c>
+      <c r="W45">
+        <v>1.2</v>
+      </c>
+      <c r="X45">
+        <v>18642</v>
+      </c>
+      <c r="Y45">
+        <v>16062000</v>
+      </c>
+      <c r="Z45">
+        <v>10749000</v>
+      </c>
+      <c r="AA45">
+        <v>57.7</v>
+      </c>
+      <c r="AB45">
+        <v>1.1</v>
+      </c>
+      <c r="AC45">
+        <v>66.90000000000001</v>
+      </c>
+      <c r="AD45">
+        <v>1.1</v>
+      </c>
+      <c r="AE45">
+        <v>8643000</v>
+      </c>
+      <c r="AF45">
+        <v>46.4</v>
+      </c>
+      <c r="AG45">
+        <v>1.1</v>
+      </c>
+      <c r="AH45">
+        <v>53.8</v>
+      </c>
+      <c r="AI45">
+        <v>1.2</v>
+      </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:35">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B46">
         <v>0.7464169774783022</v>
@@ -2172,10 +5484,82 @@
       <c r="K46">
         <v>12503</v>
       </c>
+      <c r="L46">
+        <v>2247</v>
+      </c>
+      <c r="M46">
+        <v>2109000</v>
+      </c>
+      <c r="N46">
+        <v>1443000</v>
+      </c>
+      <c r="O46">
+        <v>64.2</v>
+      </c>
+      <c r="P46">
+        <v>2.2</v>
+      </c>
+      <c r="Q46">
+        <v>68.40000000000001</v>
+      </c>
+      <c r="R46">
+        <v>2.2</v>
+      </c>
+      <c r="S46">
+        <v>1214000</v>
+      </c>
+      <c r="T46">
+        <v>54</v>
+      </c>
+      <c r="U46">
+        <v>2.3</v>
+      </c>
+      <c r="V46">
+        <v>57.6</v>
+      </c>
+      <c r="W46">
+        <v>2.4</v>
+      </c>
+      <c r="X46">
+        <v>1917</v>
+      </c>
+      <c r="Y46">
+        <v>1793000</v>
+      </c>
+      <c r="Z46">
+        <v>1138000</v>
+      </c>
+      <c r="AA46">
+        <v>59.4</v>
+      </c>
+      <c r="AB46">
+        <v>2.3</v>
+      </c>
+      <c r="AC46">
+        <v>63.5</v>
+      </c>
+      <c r="AD46">
+        <v>2.4</v>
+      </c>
+      <c r="AE46">
+        <v>1022000</v>
+      </c>
+      <c r="AF46">
+        <v>53.3</v>
+      </c>
+      <c r="AG46">
+        <v>2.4</v>
+      </c>
+      <c r="AH46">
+        <v>57</v>
+      </c>
+      <c r="AI46">
+        <v>2.4</v>
+      </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:35">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B47">
         <v>0.7606960470044406</v>
@@ -2207,10 +5591,82 @@
       <c r="K47">
         <v>4880</v>
       </c>
+      <c r="L47">
+        <v>503</v>
+      </c>
+      <c r="M47">
+        <v>497000</v>
+      </c>
+      <c r="N47">
+        <v>343000</v>
+      </c>
+      <c r="O47">
+        <v>68.09999999999999</v>
+      </c>
+      <c r="P47">
+        <v>2.9</v>
+      </c>
+      <c r="Q47">
+        <v>69</v>
+      </c>
+      <c r="R47">
+        <v>2.9</v>
+      </c>
+      <c r="S47">
+        <v>273000</v>
+      </c>
+      <c r="T47">
+        <v>54.2</v>
+      </c>
+      <c r="U47">
+        <v>3.1</v>
+      </c>
+      <c r="V47">
+        <v>54.9</v>
+      </c>
+      <c r="W47">
+        <v>3.1</v>
+      </c>
+      <c r="X47">
+        <v>496</v>
+      </c>
+      <c r="Y47">
+        <v>487000</v>
+      </c>
+      <c r="Z47">
+        <v>357000</v>
+      </c>
+      <c r="AA47">
+        <v>72</v>
+      </c>
+      <c r="AB47">
+        <v>2.5</v>
+      </c>
+      <c r="AC47">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="AD47">
+        <v>2.5</v>
+      </c>
+      <c r="AE47">
+        <v>308000</v>
+      </c>
+      <c r="AF47">
+        <v>62.1</v>
+      </c>
+      <c r="AG47">
+        <v>2.7</v>
+      </c>
+      <c r="AH47">
+        <v>63.3</v>
+      </c>
+      <c r="AI47">
+        <v>2.7</v>
+      </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:35">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B48">
         <v>0.6474450973151598</v>
@@ -2242,10 +5698,82 @@
       <c r="K48">
         <v>27819</v>
       </c>
+      <c r="L48">
+        <v>6386</v>
+      </c>
+      <c r="M48">
+        <v>5773000</v>
+      </c>
+      <c r="N48">
+        <v>4159000</v>
+      </c>
+      <c r="O48">
+        <v>65.09999999999999</v>
+      </c>
+      <c r="P48">
+        <v>2</v>
+      </c>
+      <c r="Q48">
+        <v>72</v>
+      </c>
+      <c r="R48">
+        <v>2</v>
+      </c>
+      <c r="S48">
+        <v>3319000</v>
+      </c>
+      <c r="T48">
+        <v>52</v>
+      </c>
+      <c r="U48">
+        <v>2.1</v>
+      </c>
+      <c r="V48">
+        <v>57.5</v>
+      </c>
+      <c r="W48">
+        <v>2.2</v>
+      </c>
+      <c r="X48">
+        <v>6094</v>
+      </c>
+      <c r="Y48">
+        <v>5645000</v>
+      </c>
+      <c r="Z48">
+        <v>4210000</v>
+      </c>
+      <c r="AA48">
+        <v>69.09999999999999</v>
+      </c>
+      <c r="AB48">
+        <v>1.8</v>
+      </c>
+      <c r="AC48">
+        <v>74.59999999999999</v>
+      </c>
+      <c r="AD48">
+        <v>1.7</v>
+      </c>
+      <c r="AE48">
+        <v>3778000</v>
+      </c>
+      <c r="AF48">
+        <v>62</v>
+      </c>
+      <c r="AG48">
+        <v>1.9</v>
+      </c>
+      <c r="AH48">
+        <v>66.90000000000001</v>
+      </c>
+      <c r="AI48">
+        <v>1.9</v>
+      </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:35">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B49">
         <v>0.2539974878828354</v>
@@ -2277,10 +5805,82 @@
       <c r="K49">
         <v>9313</v>
       </c>
+      <c r="L49">
+        <v>5775</v>
+      </c>
+      <c r="M49">
+        <v>5228000</v>
+      </c>
+      <c r="N49">
+        <v>3852000</v>
+      </c>
+      <c r="O49">
+        <v>66.7</v>
+      </c>
+      <c r="P49">
+        <v>2.1</v>
+      </c>
+      <c r="Q49">
+        <v>73.7</v>
+      </c>
+      <c r="R49">
+        <v>2</v>
+      </c>
+      <c r="S49">
+        <v>3234000</v>
+      </c>
+      <c r="T49">
+        <v>56</v>
+      </c>
+      <c r="U49">
+        <v>2.2</v>
+      </c>
+      <c r="V49">
+        <v>61.9</v>
+      </c>
+      <c r="W49">
+        <v>2.2</v>
+      </c>
+      <c r="X49">
+        <v>5230</v>
+      </c>
+      <c r="Y49">
+        <v>4832000</v>
+      </c>
+      <c r="Z49">
+        <v>3533000</v>
+      </c>
+      <c r="AA49">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="AB49">
+        <v>2</v>
+      </c>
+      <c r="AC49">
+        <v>73.09999999999999</v>
+      </c>
+      <c r="AD49">
+        <v>1.9</v>
+      </c>
+      <c r="AE49">
+        <v>3172000</v>
+      </c>
+      <c r="AF49">
+        <v>60.7</v>
+      </c>
+      <c r="AG49">
+        <v>2</v>
+      </c>
+      <c r="AH49">
+        <v>65.59999999999999</v>
+      </c>
+      <c r="AI49">
+        <v>2.1</v>
+      </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:35">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B50">
         <v>0.7869236544030095</v>
@@ -2312,10 +5912,82 @@
       <c r="K50">
         <v>17200</v>
       </c>
+      <c r="L50">
+        <v>1406</v>
+      </c>
+      <c r="M50">
+        <v>1384000</v>
+      </c>
+      <c r="N50">
+        <v>892000</v>
+      </c>
+      <c r="O50">
+        <v>63.4</v>
+      </c>
+      <c r="P50">
+        <v>2.8</v>
+      </c>
+      <c r="Q50">
+        <v>64.5</v>
+      </c>
+      <c r="R50">
+        <v>2.8</v>
+      </c>
+      <c r="S50">
+        <v>610000</v>
+      </c>
+      <c r="T50">
+        <v>43.4</v>
+      </c>
+      <c r="U50">
+        <v>2.9</v>
+      </c>
+      <c r="V50">
+        <v>44.1</v>
+      </c>
+      <c r="W50">
+        <v>2.9</v>
+      </c>
+      <c r="X50">
+        <v>1452</v>
+      </c>
+      <c r="Y50">
+        <v>1442000</v>
+      </c>
+      <c r="Z50">
+        <v>982000</v>
+      </c>
+      <c r="AA50">
+        <v>67.59999999999999</v>
+      </c>
+      <c r="AB50">
+        <v>2.2</v>
+      </c>
+      <c r="AC50">
+        <v>68.09999999999999</v>
+      </c>
+      <c r="AD50">
+        <v>2.2</v>
+      </c>
+      <c r="AE50">
+        <v>690000</v>
+      </c>
+      <c r="AF50">
+        <v>47.5</v>
+      </c>
+      <c r="AG50">
+        <v>2.4</v>
+      </c>
+      <c r="AH50">
+        <v>47.8</v>
+      </c>
+      <c r="AI50">
+        <v>2.4</v>
+      </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:35">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B51">
         <v>0.6915793174208524</v>
@@ -2347,10 +6019,82 @@
       <c r="K51">
         <v>48858</v>
       </c>
+      <c r="L51">
+        <v>4436</v>
+      </c>
+      <c r="M51">
+        <v>4296000</v>
+      </c>
+      <c r="N51">
+        <v>3129000</v>
+      </c>
+      <c r="O51">
+        <v>70.5</v>
+      </c>
+      <c r="P51">
+        <v>2.3</v>
+      </c>
+      <c r="Q51">
+        <v>72.8</v>
+      </c>
+      <c r="R51">
+        <v>2.2</v>
+      </c>
+      <c r="S51">
+        <v>2776000</v>
+      </c>
+      <c r="T51">
+        <v>62.6</v>
+      </c>
+      <c r="U51">
+        <v>2.4</v>
+      </c>
+      <c r="V51">
+        <v>64.59999999999999</v>
+      </c>
+      <c r="W51">
+        <v>2.4</v>
+      </c>
+      <c r="X51">
+        <v>4352</v>
+      </c>
+      <c r="Y51">
+        <v>4247000</v>
+      </c>
+      <c r="Z51">
+        <v>3318000</v>
+      </c>
+      <c r="AA51">
+        <v>76.3</v>
+      </c>
+      <c r="AB51">
+        <v>1.9</v>
+      </c>
+      <c r="AC51">
+        <v>78.09999999999999</v>
+      </c>
+      <c r="AD51">
+        <v>1.9</v>
+      </c>
+      <c r="AE51">
+        <v>3127000</v>
+      </c>
+      <c r="AF51">
+        <v>71.90000000000001</v>
+      </c>
+      <c r="AG51">
+        <v>2</v>
+      </c>
+      <c r="AH51">
+        <v>73.59999999999999</v>
+      </c>
+      <c r="AI51">
+        <v>2</v>
+      </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:35">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B52">
         <v>0.7644284262311767</v>
@@ -2381,6 +6125,78 @@
       </c>
       <c r="K52">
         <v>8237</v>
+      </c>
+      <c r="L52">
+        <v>430</v>
+      </c>
+      <c r="M52">
+        <v>422000</v>
+      </c>
+      <c r="N52">
+        <v>268000</v>
+      </c>
+      <c r="O52">
+        <v>62.4</v>
+      </c>
+      <c r="P52">
+        <v>2.9</v>
+      </c>
+      <c r="Q52">
+        <v>63.5</v>
+      </c>
+      <c r="R52">
+        <v>2.9</v>
+      </c>
+      <c r="S52">
+        <v>220000</v>
+      </c>
+      <c r="T52">
+        <v>51.2</v>
+      </c>
+      <c r="U52">
+        <v>3</v>
+      </c>
+      <c r="V52">
+        <v>52.1</v>
+      </c>
+      <c r="W52">
+        <v>3</v>
+      </c>
+      <c r="X52">
+        <v>427</v>
+      </c>
+      <c r="Y52">
+        <v>419000</v>
+      </c>
+      <c r="Z52">
+        <v>268000</v>
+      </c>
+      <c r="AA52">
+        <v>62.8</v>
+      </c>
+      <c r="AB52">
+        <v>2.6</v>
+      </c>
+      <c r="AC52">
+        <v>63.9</v>
+      </c>
+      <c r="AD52">
+        <v>2.6</v>
+      </c>
+      <c r="AE52">
+        <v>247000</v>
+      </c>
+      <c r="AF52">
+        <v>57.8</v>
+      </c>
+      <c r="AG52">
+        <v>2.6</v>
+      </c>
+      <c r="AH52">
+        <v>58.9</v>
+      </c>
+      <c r="AI52">
+        <v>2.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>